<commit_message>
TKSleep, Stop Button, Icon, Others
Implemented in this version:
Stop Button
Tksleep instead of time.sleep
Icon
Fixed last message
Organization
</commit_message>
<xml_diff>
--- a/Customer Messages Files/Customers Messages File.xlsx
+++ b/Customer Messages Files/Customers Messages File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHubPersonal\SendWhatsAppMessages\Customer Messages Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A0EB62-EE87-49D7-BBA8-0966FF329FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C40A58-D1D0-4F59-9912-A1EF8ECEA7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{569289BC-D768-472D-9366-0DDE05FEA49D}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <dimension ref="A1:H166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +557,7 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">"Dados não relevantes aqui "&amp;TEXT(RANDBETWEEN(1,10),"00")</f>
-        <v>Dados não relevantes aqui 02</v>
+        <v>Dados não relevantes aqui 03</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -573,7 +573,7 @@
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B18" ca="1" si="0">"Dados não relevantes aqui "&amp;TEXT(RANDBETWEEN(1,10),"00")</f>
-        <v>Dados não relevantes aqui 01</v>
+        <v>Dados não relevantes aqui 04</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -592,7 +592,7 @@
       </c>
       <c r="B4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 01</v>
+        <v>Dados não relevantes aqui 09</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="B5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 07</v>
+        <v>Dados não relevantes aqui 04</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -621,7 +621,7 @@
       </c>
       <c r="B6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 02</v>
+        <v>Dados não relevantes aqui 04</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -640,7 +640,7 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 06</v>
+        <v>Dados não relevantes aqui 07</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -656,7 +656,7 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 03</v>
+        <v>Dados não relevantes aqui 06</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -669,7 +669,7 @@
       </c>
       <c r="B9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 03</v>
+        <v>Dados não relevantes aqui 04</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -682,7 +682,7 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 01</v>
+        <v>Dados não relevantes aqui 10</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -698,7 +698,7 @@
       </c>
       <c r="B11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 03</v>
+        <v>Dados não relevantes aqui 01</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -714,13 +714,13 @@
       </c>
       <c r="B12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 05</v>
+        <v>Dados não relevantes aqui 09</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="1" t="str">
-        <f t="shared" ref="D12:D18" si="1">"Mensagem de Teste para "&amp;A12</f>
+        <f t="shared" ref="D12:D17" si="1">"Mensagem de Teste para "&amp;A12</f>
         <v>Mensagem de Teste para João message</v>
       </c>
     </row>
@@ -730,7 +730,7 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 04</v>
+        <v>Dados não relevantes aqui 09</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -746,7 +746,7 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 02</v>
+        <v>Dados não relevantes aqui 10</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
@@ -762,7 +762,7 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 07</v>
+        <v>Dados não relevantes aqui 08</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -794,7 +794,7 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 06</v>
+        <v>Dados não relevantes aqui 02</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
@@ -810,7 +810,7 @@
       </c>
       <c r="B18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dados não relevantes aqui 07</v>
+        <v>Dados não relevantes aqui 05</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Using Tk Variables ilo globals
</commit_message>
<xml_diff>
--- a/Customer Messages Files/Customers Messages File.xlsx
+++ b/Customer Messages Files/Customers Messages File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHubPersonal\SendWhatsAppMessages\Customer Messages Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6A6123-9C64-4F05-A210-BB6DA2AEAC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F44FE8-B699-4C12-B4A9-23CF25026D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{569289BC-D768-472D-9366-0DDE05FEA49D}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Pablo</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Garbage</t>
+  </si>
+  <si>
+    <t>55 (71) 9101-3035</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
   <dimension ref="A1:G166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="str">
         <f>"Testing Message for "&amp;A2</f>
@@ -567,7 +570,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="str">
         <f>"Testing Message for "&amp;A3</f>
@@ -582,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -603,7 +606,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>"Testing Message for "&amp;A6</f>
@@ -617,6 +620,9 @@
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C7" s="3" t="str">
         <f>"Testing Message for "&amp;A7</f>
         <v>Testing Message for José wrong number</v>
@@ -627,7 +633,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -636,7 +642,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -645,7 +651,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>"Testing Message for "&amp;A10</f>

</xml_diff>

<commit_message>
Added Start Time, Estimated End Time and Percent
</commit_message>
<xml_diff>
--- a/Customer Messages Files/Customers Messages File.xlsx
+++ b/Customer Messages Files/Customers Messages File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHubPersonal\SendWhatsAppMessages\Customer Messages Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F44FE8-B699-4C12-B4A9-23CF25026D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDB3423-3908-4434-8BE1-B521282F0327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{569289BC-D768-472D-9366-0DDE05FEA49D}"/>
+    <workbookView xWindow="1170" yWindow="4665" windowWidth="21600" windowHeight="12735" xr2:uid="{569289BC-D768-472D-9366-0DDE05FEA49D}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIENTES" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Pablo</t>
   </si>
@@ -112,7 +112,7 @@
     <t>Garbage</t>
   </si>
   <si>
-    <t>55 (71) 9101-3035</t>
+    <t>Empty number</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:G166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="str">
         <f>"Testing Message for "&amp;A2</f>
@@ -570,7 +570,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="str">
         <f>"Testing Message for "&amp;A3</f>
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -606,7 +606,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>"Testing Message for "&amp;A6</f>
@@ -633,7 +633,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -642,7 +642,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -651,7 +651,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>"Testing Message for "&amp;A10</f>
@@ -662,9 +662,8 @@
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3" t="str">
-        <f>"Testing Message for "&amp;A11</f>
-        <v>Testing Message for Maria Wrong number</v>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -683,12 +682,8 @@
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3" t="str">
-        <f>"Testing Message for "&amp;A13</f>
-        <v>Testing Message for Jõao wrong number</v>
+      <c r="C13" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improved Information to User
Percent of messages sent and failed
Improved results file (removed message field)
</commit_message>
<xml_diff>
--- a/Customer Messages Files/Customers Messages File.xlsx
+++ b/Customer Messages Files/Customers Messages File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHubPersonal\SendWhatsAppMessages\Customer Messages Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDB3423-3908-4434-8BE1-B521282F0327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC813D9-576C-45D8-8446-67DBC1DDF4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="4665" windowWidth="21600" windowHeight="12735" xr2:uid="{569289BC-D768-472D-9366-0DDE05FEA49D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{569289BC-D768-472D-9366-0DDE05FEA49D}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIENTES" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Pablo</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Maria Wrong number</t>
   </si>
   <si>
-    <t>Columna Ocupada Al Pedo</t>
-  </si>
-  <si>
     <t>João message</t>
   </si>
   <si>
@@ -109,17 +106,20 @@
     <t>Sicrano</t>
   </si>
   <si>
+    <t>Empty number</t>
+  </si>
+  <si>
+    <t>55(71) 9101-3035</t>
+  </si>
+  <si>
     <t>Garbage</t>
-  </si>
-  <si>
-    <t>Empty number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +135,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,11 +165,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -169,6 +193,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3134E6-AFCE-4D07-881D-E8F9A6212C6E}">
-  <dimension ref="A1:G166"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,10 +566,11 @@
     <col min="1" max="1" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -549,38 +580,37 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="B2" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="str">
         <f>"Testing Message for "&amp;A2</f>
         <v>Testing Message for Pablo</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+      <c r="B3" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="str">
         <f>"Testing Message for "&amp;A3</f>
         <v>Testing Message for Pedro with valid message</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -589,7 +619,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -600,23 +630,23 @@
         <f>"Testing Message for "&amp;A5</f>
         <v>Testing Message for Pedro Wrong Number</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>"Testing Message for "&amp;A6</f>
         <v>Testing Message for José valid message</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -628,7 +658,7 @@
         <v>Testing Message for José wrong number</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -637,7 +667,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -646,7 +676,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -657,38 +687,40 @@
         <f>"Testing Message for "&amp;A10</f>
         <v>Testing Message for Maria with message</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C12" s="3" t="str">
         <f>"Testing Message for "&amp;A12</f>
         <v>Testing Message for João message</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
@@ -700,9 +732,9 @@
  https://www.youtube.com/</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
@@ -713,10 +745,11 @@
         <v>A very long text message with a link here for Fulano
  https://www.google.com/</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>5</v>
@@ -726,9 +759,9 @@
         <v>Testing Message for Beltrano</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
@@ -737,13 +770,14 @@
         <f>"Testing Message for "&amp;A17</f>
         <v>Testing Message for Sultano</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C18" s="4" t="str">
         <f>"A very long text message with a link here for "&amp;A18&amp;"
@@ -752,46 +786,46 @@
  https://www.instagram.com/</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>